<commit_message>
Update accident data and map simulation
Added a new accident record to accident_data.csv and updated accident_report.xlsx. Updated road_accident_map_simulation.html to use a new map element ID and variable, likely reflecting changes in the mapping library or data structure.
</commit_message>
<xml_diff>
--- a/accident_report.xlsx
+++ b/accident_report.xlsx
@@ -656,7 +656,7 @@
     <row r="4">
       <c r="A4" s="3" t="inlineStr">
         <is>
-          <t>Vehicle-pedestrian collision</t>
+          <t>Head-on collision</t>
         </is>
       </c>
       <c r="B4" s="3" t="inlineStr">
@@ -666,7 +666,7 @@
       </c>
       <c r="C4" s="3" t="inlineStr">
         <is>
-          <t>2.91 seconds</t>
+          <t>2.08 seconds</t>
         </is>
       </c>
       <c r="D4" s="3" t="inlineStr">
@@ -680,24 +680,28 @@
         </is>
       </c>
       <c r="F4" s="3" t="n">
-        <v>1364</v>
+        <v>1316</v>
       </c>
       <c r="G4" s="3" t="inlineStr">
         <is>
-          <t>63.5</t>
-        </is>
-      </c>
-      <c r="H4" s="3" t="inlineStr"/>
-      <c r="I4" s="3" t="inlineStr"/>
-      <c r="J4" s="3" t="inlineStr"/>
-      <c r="K4" s="3" t="inlineStr">
-        <is>
-          <t>Pedestrian</t>
-        </is>
-      </c>
-      <c r="L4" s="3" t="n">
-        <v>58</v>
-      </c>
+          <t>83.6</t>
+        </is>
+      </c>
+      <c r="H4" s="3" t="inlineStr">
+        <is>
+          <t>Car 2</t>
+        </is>
+      </c>
+      <c r="I4" s="3" t="n">
+        <v>1451</v>
+      </c>
+      <c r="J4" s="3" t="inlineStr">
+        <is>
+          <t>-80.8</t>
+        </is>
+      </c>
+      <c r="K4" s="3" t="inlineStr"/>
+      <c r="L4" s="3" t="inlineStr"/>
       <c r="M4" s="3" t="inlineStr">
         <is>
           <t>wet</t>
@@ -714,21 +718,21 @@
         </is>
       </c>
       <c r="P4" s="3" t="n">
-        <v>15</v>
+        <v>180</v>
       </c>
       <c r="Q4" s="3" t="inlineStr">
         <is>
-          <t>2.91</t>
+          <t>2.08</t>
         </is>
       </c>
       <c r="R4" s="3" t="inlineStr">
         <is>
-          <t>107857.46</t>
+          <t>3213773.80</t>
         </is>
       </c>
       <c r="S4" s="3" t="inlineStr">
         <is>
-          <t>moderate</t>
+          <t>severe</t>
         </is>
       </c>
       <c r="T4" s="3" t="n">
@@ -741,11 +745,11 @@
       </c>
       <c r="V4" s="3" t="inlineStr">
         <is>
-          <t>- Install additional street lights
-- Weather-based speed limit adjustments
-- Install breathalyzer devices
-- Pedestrian safety education
-- Stricter DUI checkpoints</t>
+          <t>- Solar-powered lighting solutions
+- Public awareness campaigns on drinking and driving
+- Install anti-skid road surfaces
+- One-way traffic in narrow roads
+- Install breathalyzer devices</t>
         </is>
       </c>
       <c r="W4" s="3" t="inlineStr">
@@ -755,7 +759,7 @@
       </c>
       <c r="X4" s="3" t="inlineStr">
         <is>
-          <t>12.1% of historical accidents in Main Highway share moderate severity.</t>
+          <t>85.3% of historical accidents in Main Highway share severe severity.</t>
         </is>
       </c>
       <c r="Y4" s="3" t="inlineStr">
@@ -765,32 +769,32 @@
       </c>
       <c r="Z4" s="3" t="inlineStr">
         <is>
-          <t>moderate</t>
+          <t>severe</t>
         </is>
       </c>
       <c r="AA4" s="3" t="inlineStr">
         <is>
-          <t>moderate</t>
+          <t>severe</t>
         </is>
       </c>
       <c r="AB4" s="3" t="inlineStr">
         <is>
-          <t>107857.46</t>
+          <t>3213773.80</t>
         </is>
       </c>
       <c r="AC4" s="3" t="inlineStr">
         <is>
-          <t>80893.10</t>
+          <t>2607714.87</t>
         </is>
       </c>
       <c r="AD4" s="3" t="inlineStr">
         <is>
-          <t>25.00%</t>
+          <t>18.86%</t>
         </is>
       </c>
       <c r="AE4" s="3" t="inlineStr">
         <is>
-          <t>0.20 (Baseline 10.00, Intervention 9.80)</t>
+          <t>0.00 (Baseline 10.00, Intervention 10.00)</t>
         </is>
       </c>
       <c r="AF4" s="3" t="inlineStr">
@@ -800,7 +804,7 @@
       </c>
       <c r="AG4" s="3" t="inlineStr">
         <is>
-          <t>9.80</t>
+          <t>10.00</t>
         </is>
       </c>
     </row>

</xml_diff>